<commit_message>
Fix: add status to report
</commit_message>
<xml_diff>
--- a/templates/report_template.xlsx
+++ b/templates/report_template.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15540" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="114">
   <si>
     <t>Order Date</t>
   </si>
@@ -360,6 +360,12 @@
   </si>
   <si>
     <t>${table:rawData.cInfo.floor}</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>${table:rawData.status2}</t>
   </si>
 </sst>
 </file>
@@ -728,36 +734,37 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:BD2"/>
+  <dimension ref="A1:BE2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H5" sqref="H5"/>
+      <selection pane="bottomLeft" activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="26.33203125" customWidth="1"/>
     <col min="2" max="2" width="19.6640625" customWidth="1"/>
-    <col min="3" max="3" width="22.1640625" customWidth="1"/>
-    <col min="4" max="4" width="25.5" customWidth="1"/>
-    <col min="5" max="5" width="27" customWidth="1"/>
-    <col min="6" max="6" width="13" customWidth="1"/>
-    <col min="7" max="7" width="28.33203125" customWidth="1"/>
-    <col min="8" max="8" width="29.1640625" customWidth="1"/>
-    <col min="9" max="9" width="16.1640625" customWidth="1"/>
-    <col min="10" max="10" width="29.1640625" customWidth="1"/>
-    <col min="11" max="12" width="11.5" customWidth="1"/>
-    <col min="13" max="13" width="17.6640625" customWidth="1"/>
-    <col min="14" max="14" width="19.33203125" customWidth="1"/>
-    <col min="15" max="15" width="19.6640625" customWidth="1"/>
-    <col min="16" max="17" width="30.5" customWidth="1"/>
-    <col min="18" max="18" width="24.33203125" customWidth="1"/>
-    <col min="19" max="19" width="20" customWidth="1"/>
-    <col min="20" max="20" width="14.33203125" customWidth="1"/>
+    <col min="3" max="3" width="23.33203125" customWidth="1"/>
+    <col min="4" max="4" width="22.1640625" customWidth="1"/>
+    <col min="5" max="5" width="25.5" customWidth="1"/>
+    <col min="6" max="6" width="27" customWidth="1"/>
+    <col min="7" max="7" width="13" customWidth="1"/>
+    <col min="8" max="8" width="28.33203125" customWidth="1"/>
+    <col min="9" max="9" width="29.1640625" customWidth="1"/>
+    <col min="10" max="10" width="16.1640625" customWidth="1"/>
+    <col min="11" max="11" width="29.1640625" customWidth="1"/>
+    <col min="12" max="13" width="11.5" customWidth="1"/>
+    <col min="14" max="14" width="17.6640625" customWidth="1"/>
+    <col min="15" max="15" width="19.33203125" customWidth="1"/>
+    <col min="16" max="16" width="19.6640625" customWidth="1"/>
+    <col min="17" max="18" width="30.5" customWidth="1"/>
+    <col min="19" max="19" width="24.33203125" customWidth="1"/>
+    <col min="20" max="20" width="20" customWidth="1"/>
+    <col min="21" max="21" width="14.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:56" s="4" customFormat="1" ht="24" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:57" s="4" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>28</v>
       </c>
@@ -765,169 +772,172 @@
         <v>27</v>
       </c>
       <c r="C1" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="D1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="E1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="F1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="G1" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="H1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="I1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="J1" s="4" t="s">
         <v>110</v>
       </c>
-      <c r="J1" s="4" t="s">
+      <c r="K1" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="K1" s="4" t="s">
+      <c r="L1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="L1" s="4" t="s">
+      <c r="M1" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="M1" s="4" t="s">
+      <c r="N1" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="N1" s="4" t="s">
+      <c r="O1" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="O1" s="4" t="s">
+      <c r="P1" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="P1" s="4" t="s">
+      <c r="Q1" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="Q1" s="6" t="s">
+      <c r="R1" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="R1" s="6" t="s">
+      <c r="S1" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="S1" s="6" t="s">
+      <c r="T1" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="T1" s="6" t="s">
+      <c r="U1" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="U1" s="6" t="s">
+      <c r="V1" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="V1" s="6" t="s">
+      <c r="W1" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="W1" s="6" t="s">
+      <c r="X1" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="X1" s="6" t="s">
+      <c r="Y1" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="Y1" s="6" t="s">
+      <c r="Z1" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="Z1" s="6" t="s">
+      <c r="AA1" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="AA1" s="6" t="s">
+      <c r="AB1" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="AB1" s="6" t="s">
+      <c r="AC1" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="AC1" s="6" t="s">
+      <c r="AD1" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="AD1" s="6" t="s">
+      <c r="AE1" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="AE1" s="6" t="s">
+      <c r="AF1" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="AF1" s="6" t="s">
+      <c r="AG1" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="AG1" s="6" t="s">
+      <c r="AH1" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="AH1" s="6" t="s">
+      <c r="AI1" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="AI1" s="6" t="s">
+      <c r="AJ1" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="AJ1" s="6" t="s">
+      <c r="AK1" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="AK1" s="6" t="s">
+      <c r="AL1" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="AL1" s="6" t="s">
+      <c r="AM1" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="AM1" s="6" t="s">
+      <c r="AN1" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="AN1" s="6" t="s">
+      <c r="AO1" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="AO1" s="6" t="s">
+      <c r="AP1" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="AP1" s="6" t="s">
+      <c r="AQ1" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="AQ1" s="6" t="s">
+      <c r="AR1" s="6" t="s">
         <v>60</v>
       </c>
-      <c r="AR1" s="6" t="s">
+      <c r="AS1" s="6" t="s">
         <v>61</v>
       </c>
-      <c r="AS1" s="6" t="s">
+      <c r="AT1" s="6" t="s">
         <v>64</v>
       </c>
-      <c r="AT1" s="6" t="s">
+      <c r="AU1" s="6" t="s">
         <v>65</v>
       </c>
-      <c r="AU1" s="6" t="s">
+      <c r="AV1" s="6" t="s">
         <v>62</v>
       </c>
-      <c r="AV1" s="6" t="s">
+      <c r="AW1" s="6" t="s">
         <v>63</v>
       </c>
-      <c r="AW1" s="6" t="s">
+      <c r="AX1" s="6" t="s">
         <v>66</v>
       </c>
-      <c r="AX1" s="6" t="s">
+      <c r="AY1" s="6" t="s">
         <v>67</v>
       </c>
-      <c r="AY1" s="6" t="s">
+      <c r="AZ1" s="6" t="s">
         <v>68</v>
       </c>
-      <c r="AZ1" s="6" t="s">
+      <c r="BA1" s="6" t="s">
         <v>69</v>
       </c>
-      <c r="BA1" s="6" t="s">
+      <c r="BB1" s="6" t="s">
         <v>70</v>
       </c>
-      <c r="BB1" s="6" t="s">
+      <c r="BC1" s="6" t="s">
         <v>71</v>
       </c>
-      <c r="BC1" s="6" t="s">
+      <c r="BD1" s="6" t="s">
         <v>72</v>
       </c>
-      <c r="BD1" s="6" t="s">
+      <c r="BE1" s="6" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="2" spans="1:56" s="3" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:57" s="3" customFormat="1" ht="19" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>24</v>
       </c>
@@ -935,165 +945,168 @@
         <v>29</v>
       </c>
       <c r="C2" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="D2" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="E2" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="F2" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="G2" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="H2" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="H2" s="3" t="s">
+      <c r="I2" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="I2" s="3" t="s">
+      <c r="J2" s="3" t="s">
         <v>111</v>
       </c>
-      <c r="J2" s="3" t="s">
+      <c r="K2" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="K2" s="3" t="s">
+      <c r="L2" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="L2" s="3" t="s">
+      <c r="M2" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="M2" s="3" t="s">
+      <c r="N2" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="N2" s="5" t="s">
+      <c r="O2" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="O2" s="3" t="s">
+      <c r="P2" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="P2" s="3" t="s">
+      <c r="Q2" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="Q2" s="3" t="s">
+      <c r="R2" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="R2" s="3" t="s">
+      <c r="S2" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="S2" s="3" t="s">
+      <c r="T2" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="T2" s="3" t="s">
+      <c r="U2" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="U2" s="3" t="s">
+      <c r="V2" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="V2" s="3" t="s">
+      <c r="W2" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="W2" s="3" t="s">
+      <c r="X2" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="X2" s="3" t="s">
+      <c r="Y2" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="Y2" s="3" t="s">
+      <c r="Z2" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="Z2" s="3" t="s">
+      <c r="AA2" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="AA2" s="3" t="s">
+      <c r="AB2" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="AB2" s="3" t="s">
+      <c r="AC2" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="AC2" s="3" t="s">
+      <c r="AD2" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="AD2" s="3" t="s">
+      <c r="AE2" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="AE2" s="3" t="s">
+      <c r="AF2" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="AF2" s="3" t="s">
+      <c r="AG2" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="AG2" s="3" t="s">
+      <c r="AH2" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="AH2" s="3" t="s">
+      <c r="AI2" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="AI2" s="3" t="s">
+      <c r="AJ2" s="3" t="s">
         <v>88</v>
       </c>
-      <c r="AJ2" s="3" t="s">
+      <c r="AK2" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="AK2" s="3" t="s">
+      <c r="AL2" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="AL2" s="3" t="s">
+      <c r="AM2" s="3" t="s">
         <v>91</v>
       </c>
-      <c r="AM2" s="3" t="s">
+      <c r="AN2" s="3" t="s">
         <v>92</v>
       </c>
-      <c r="AN2" s="3" t="s">
+      <c r="AO2" s="3" t="s">
         <v>93</v>
       </c>
-      <c r="AO2" s="3" t="s">
+      <c r="AP2" s="3" t="s">
         <v>94</v>
       </c>
-      <c r="AP2" s="3" t="s">
+      <c r="AQ2" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="AQ2" s="3" t="s">
+      <c r="AR2" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="AR2" s="3" t="s">
+      <c r="AS2" s="3" t="s">
         <v>97</v>
       </c>
-      <c r="AS2" s="3" t="s">
+      <c r="AT2" s="3" t="s">
         <v>98</v>
       </c>
-      <c r="AT2" s="3" t="s">
+      <c r="AU2" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="AU2" s="3" t="s">
+      <c r="AV2" s="3" t="s">
         <v>100</v>
       </c>
-      <c r="AV2" s="3" t="s">
+      <c r="AW2" s="3" t="s">
         <v>101</v>
       </c>
-      <c r="AW2" s="3" t="s">
+      <c r="AX2" s="3" t="s">
         <v>102</v>
       </c>
-      <c r="AX2" s="3" t="s">
+      <c r="AY2" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="AY2" s="3" t="s">
+      <c r="AZ2" s="3" t="s">
         <v>104</v>
       </c>
-      <c r="AZ2" s="3" t="s">
+      <c r="BA2" s="3" t="s">
         <v>105</v>
       </c>
-      <c r="BA2" s="3" t="s">
+      <c r="BB2" s="3" t="s">
         <v>106</v>
       </c>
-      <c r="BB2" s="3" t="s">
+      <c r="BC2" s="3" t="s">
         <v>107</v>
       </c>
-      <c r="BC2" s="3" t="s">
+      <c r="BD2" s="3" t="s">
         <v>108</v>
       </c>
-      <c r="BD2" s="3" t="s">
+      <c r="BE2" s="3" t="s">
         <v>109</v>
       </c>
     </row>

</xml_diff>